<commit_message>
el codigo no da, no funciona
</commit_message>
<xml_diff>
--- a/planilla de almendras para QR.xlsx
+++ b/planilla de almendras para QR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\APK QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6BCCFB-E7C0-46EF-8050-0911EA5823A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A586CE6-D3CB-479B-A0CE-C387A6778F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -4320,7 +4320,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10904679" y="2424544"/>
+          <a:off x="10918286" y="2444337"/>
           <a:ext cx="2395685" cy="2490933"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4360,7 +4360,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10904679" y="5351317"/>
+          <a:off x="10918286" y="5369872"/>
           <a:ext cx="2395685" cy="2490933"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -19816,8 +19816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J61"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21481,8 +21481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
QR retorna los datos de: ID, Beneficiario, Comunidad, GPS 1, GPS 2
</commit_message>
<xml_diff>
--- a/planilla de almendras para QR.xlsx
+++ b/planilla de almendras para QR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\APK QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6BCCFB-E7C0-46EF-8050-0911EA5823A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577862FC-0486-4A3F-B2BF-6D08BF3D24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -19816,8 +19816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J61"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21481,7 +21481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se añadio una nueva columa a la tabla de excel solo a una hoja, falta hacer es para las demas hojas y tambien poner las fechas
</commit_message>
<xml_diff>
--- a/planilla de almendras para QR.xlsx
+++ b/planilla de almendras para QR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\APK QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577862FC-0486-4A3F-B2BF-6D08BF3D24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C7580-68E3-4519-AC6F-1794DE8C3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="485">
   <si>
     <t>Resumen de las comunidades - Productores y numero de plantas georeferenciadas.</t>
   </si>
@@ -1480,14 +1480,18 @@
   </si>
   <si>
     <t>CA_JB_170</t>
+  </si>
+  <si>
+    <t>Fecha Plantaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1897,7 +1901,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2082,7 +2086,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2101,6 +2111,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2125,7 +2138,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2165,7 +2178,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2205,7 +2218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2245,7 +2258,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2285,7 +2298,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2325,7 +2338,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2365,7 +2378,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2405,7 +2418,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2445,7 +2458,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2485,7 +2498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2525,7 +2538,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2565,7 +2578,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2605,7 +2618,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2645,7 +2658,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2685,7 +2698,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2725,7 +2738,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2765,7 +2778,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2805,7 +2818,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2845,7 +2858,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2885,7 +2898,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2925,7 +2938,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2965,7 +2978,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3005,7 +3018,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3045,7 +3058,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3085,7 +3098,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3125,7 +3138,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3165,7 +3178,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3205,7 +3218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3245,7 +3258,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3285,7 +3298,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3325,7 +3338,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3365,7 +3378,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3405,7 +3418,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3445,7 +3458,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3485,7 +3498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3525,7 +3538,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3565,7 +3578,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3605,7 +3618,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3645,7 +3658,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3685,7 +3698,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3725,7 +3738,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3765,7 +3778,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3805,7 +3818,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3845,7 +3858,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3885,7 +3898,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3925,7 +3938,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3965,7 +3978,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>214313</xdr:rowOff>
@@ -19814,10 +19827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:J61"/>
+  <dimension ref="A2:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19826,14 +19839,14 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="48.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="5" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -19844,8 +19857,9 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -19856,8 +19870,9 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="13" t="s">
         <v>16</v>
@@ -19866,14 +19881,15 @@
       <c r="D4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="88"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="24" t="s">
         <v>17</v>
@@ -19883,13 +19899,14 @@
         <v>6</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="84"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="88"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="13" t="s">
         <v>18</v>
@@ -19898,14 +19915,15 @@
       <c r="D6" s="13">
         <v>47</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="85"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -19915,13 +19933,14 @@
       <c r="E7" s="27">
         <v>8314</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -19932,8 +19951,9 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="30" t="s">
         <v>20</v>
@@ -19948,20 +19968,23 @@
         <v>23</v>
       </c>
       <c r="F9" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="H9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="I9" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="78" t="s">
+      <c r="J9" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79"/>
       <c r="B10" s="28">
         <v>1</v>
@@ -19975,19 +19998,22 @@
       <c r="E10" s="28">
         <v>8314823</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="94">
+        <v>45485</v>
+      </c>
+      <c r="G10" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="79"/>
-    </row>
-    <row r="11" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="60"/>
+      <c r="K10" s="79"/>
+    </row>
+    <row r="11" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79"/>
       <c r="B11" s="21">
         <v>2</v>
@@ -20001,17 +20027,20 @@
       <c r="E11" s="21">
         <v>8314823</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="94">
+        <v>45486</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="60"/>
-      <c r="J11" s="79"/>
-    </row>
-    <row r="12" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="60"/>
+      <c r="K11" s="79"/>
+    </row>
+    <row r="12" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79"/>
       <c r="B12" s="21">
         <v>3</v>
@@ -20025,17 +20054,20 @@
       <c r="E12" s="21">
         <v>8314821</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21" t="s">
+      <c r="F12" s="94">
+        <v>45487</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="I12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="79"/>
-    </row>
-    <row r="13" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="60"/>
+      <c r="K12" s="79"/>
+    </row>
+    <row r="13" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79"/>
       <c r="B13" s="21">
         <v>4</v>
@@ -20049,15 +20081,18 @@
       <c r="E13" s="21">
         <v>8314821</v>
       </c>
-      <c r="F13" s="21"/>
+      <c r="F13" s="94">
+        <v>45488</v>
+      </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="60"/>
-      <c r="J13" s="79"/>
-    </row>
-    <row r="14" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="60"/>
+      <c r="K13" s="79"/>
+    </row>
+    <row r="14" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79"/>
       <c r="B14" s="21">
         <v>5</v>
@@ -20071,15 +20106,18 @@
       <c r="E14" s="21">
         <v>8314820</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="94">
+        <v>45489</v>
+      </c>
       <c r="G14" s="21"/>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="79"/>
-    </row>
-    <row r="15" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="60"/>
+      <c r="K14" s="79"/>
+    </row>
+    <row r="15" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79"/>
       <c r="B15" s="21">
         <v>6</v>
@@ -20093,15 +20131,18 @@
       <c r="E15" s="21">
         <v>8314819</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="84">
+        <v>45490</v>
+      </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="60"/>
-      <c r="J15" s="79"/>
-    </row>
-    <row r="16" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="60"/>
+      <c r="K15" s="79"/>
+    </row>
+    <row r="16" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="79"/>
       <c r="B16" s="21">
         <v>7</v>
@@ -20117,13 +20158,14 @@
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="79"/>
-    </row>
-    <row r="17" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="60"/>
+      <c r="K16" s="79"/>
+    </row>
+    <row r="17" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="79"/>
       <c r="B17" s="21">
         <v>8</v>
@@ -20139,13 +20181,14 @@
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="60"/>
-      <c r="J17" s="79"/>
-    </row>
-    <row r="18" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="60"/>
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="79"/>
       <c r="B18" s="21">
         <v>9</v>
@@ -20161,13 +20204,14 @@
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="21"/>
+      <c r="I18" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="79"/>
-    </row>
-    <row r="19" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="60"/>
+      <c r="K18" s="79"/>
+    </row>
+    <row r="19" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="79"/>
       <c r="B19" s="21">
         <v>10</v>
@@ -20183,13 +20227,14 @@
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="79"/>
-    </row>
-    <row r="20" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="21"/>
+      <c r="K19" s="79"/>
+    </row>
+    <row r="20" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="79"/>
       <c r="B20" s="21">
         <v>11</v>
@@ -20205,13 +20250,14 @@
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="21"/>
+      <c r="I20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="79"/>
-    </row>
-    <row r="21" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="21"/>
+      <c r="K20" s="79"/>
+    </row>
+    <row r="21" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="79"/>
       <c r="B21" s="21">
         <v>12</v>
@@ -20227,13 +20273,14 @@
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="21"/>
+      <c r="I21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="79"/>
-    </row>
-    <row r="22" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="21"/>
+      <c r="K21" s="79"/>
+    </row>
+    <row r="22" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="79"/>
       <c r="B22" s="21">
         <v>13</v>
@@ -20249,13 +20296,14 @@
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="21"/>
+      <c r="I22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="79"/>
-    </row>
-    <row r="23" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="21"/>
+      <c r="K22" s="79"/>
+    </row>
+    <row r="23" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="79"/>
       <c r="B23" s="21">
         <v>14</v>
@@ -20271,13 +20319,14 @@
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="21"/>
+      <c r="I23" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="79"/>
-    </row>
-    <row r="24" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="21"/>
+      <c r="K23" s="79"/>
+    </row>
+    <row r="24" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="79"/>
       <c r="B24" s="21">
         <v>15</v>
@@ -20293,13 +20342,14 @@
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="21"/>
+      <c r="I24" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="79"/>
-    </row>
-    <row r="25" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="21"/>
+      <c r="K24" s="79"/>
+    </row>
+    <row r="25" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="79"/>
       <c r="B25" s="21">
         <v>16</v>
@@ -20315,13 +20365,14 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="21"/>
+      <c r="I25" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="79"/>
-    </row>
-    <row r="26" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="21"/>
+      <c r="K25" s="79"/>
+    </row>
+    <row r="26" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="79"/>
       <c r="B26" s="21">
         <v>17</v>
@@ -20337,13 +20388,14 @@
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="21"/>
+      <c r="I26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="21"/>
-      <c r="J26" s="79"/>
-    </row>
-    <row r="27" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="21"/>
+      <c r="K26" s="79"/>
+    </row>
+    <row r="27" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="79"/>
       <c r="B27" s="21">
         <v>18</v>
@@ -20359,13 +20411,14 @@
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="21"/>
+      <c r="I27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="79"/>
-    </row>
-    <row r="28" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="21"/>
+      <c r="K27" s="79"/>
+    </row>
+    <row r="28" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="79"/>
       <c r="B28" s="21">
         <v>19</v>
@@ -20381,13 +20434,14 @@
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="21"/>
+      <c r="I28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="79"/>
-    </row>
-    <row r="29" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="21"/>
+      <c r="K28" s="79"/>
+    </row>
+    <row r="29" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="79"/>
       <c r="B29" s="21">
         <v>20</v>
@@ -20403,13 +20457,14 @@
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="21"/>
+      <c r="I29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="79"/>
-    </row>
-    <row r="30" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="21"/>
+      <c r="K29" s="79"/>
+    </row>
+    <row r="30" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="79"/>
       <c r="B30" s="21">
         <v>21</v>
@@ -20425,13 +20480,14 @@
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="21"/>
+      <c r="I30" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="79"/>
-    </row>
-    <row r="31" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="21"/>
+      <c r="K30" s="79"/>
+    </row>
+    <row r="31" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="79"/>
       <c r="B31" s="21">
         <v>22</v>
@@ -20447,13 +20503,14 @@
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="21"/>
+      <c r="I31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="79"/>
-    </row>
-    <row r="32" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="21"/>
+      <c r="K31" s="79"/>
+    </row>
+    <row r="32" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="79"/>
       <c r="B32" s="21">
         <v>23</v>
@@ -20469,13 +20526,14 @@
       </c>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="21"/>
+      <c r="I32" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="79"/>
-    </row>
-    <row r="33" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="21"/>
+      <c r="K32" s="79"/>
+    </row>
+    <row r="33" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="79"/>
       <c r="B33" s="21">
         <v>24</v>
@@ -20491,13 +20549,14 @@
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="21"/>
+      <c r="I33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="79"/>
-    </row>
-    <row r="34" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="21"/>
+      <c r="K33" s="79"/>
+    </row>
+    <row r="34" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="79"/>
       <c r="B34" s="21">
         <v>25</v>
@@ -20513,13 +20572,14 @@
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="21"/>
+      <c r="I34" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="79"/>
-    </row>
-    <row r="35" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="21"/>
+      <c r="K34" s="79"/>
+    </row>
+    <row r="35" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="79"/>
       <c r="B35" s="21">
         <v>26</v>
@@ -20535,13 +20595,14 @@
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="21"/>
+      <c r="I35" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="79"/>
-    </row>
-    <row r="36" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="21"/>
+      <c r="K35" s="79"/>
+    </row>
+    <row r="36" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="79"/>
       <c r="B36" s="21">
         <v>27</v>
@@ -20557,13 +20618,14 @@
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="21"/>
+      <c r="I36" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="79"/>
-    </row>
-    <row r="37" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="21"/>
+      <c r="K36" s="79"/>
+    </row>
+    <row r="37" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="79"/>
       <c r="B37" s="21">
         <v>28</v>
@@ -20579,13 +20641,14 @@
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="21" t="s">
+      <c r="H37" s="21"/>
+      <c r="I37" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="79"/>
-    </row>
-    <row r="38" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="21"/>
+      <c r="K37" s="79"/>
+    </row>
+    <row r="38" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="79"/>
       <c r="B38" s="21">
         <v>29</v>
@@ -20601,13 +20664,14 @@
       </c>
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="21"/>
+      <c r="I38" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="79"/>
-    </row>
-    <row r="39" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="21"/>
+      <c r="K38" s="79"/>
+    </row>
+    <row r="39" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="79"/>
       <c r="B39" s="21">
         <v>30</v>
@@ -20623,13 +20687,14 @@
       </c>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="21"/>
+      <c r="I39" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="79"/>
-    </row>
-    <row r="40" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="21"/>
+      <c r="K39" s="79"/>
+    </row>
+    <row r="40" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="79"/>
       <c r="B40" s="21">
         <v>31</v>
@@ -20645,13 +20710,14 @@
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="21"/>
+      <c r="I40" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="79"/>
-    </row>
-    <row r="41" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="21"/>
+      <c r="K40" s="79"/>
+    </row>
+    <row r="41" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="79"/>
       <c r="B41" s="21">
         <v>32</v>
@@ -20667,13 +20733,14 @@
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="21"/>
+      <c r="I41" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="79"/>
-    </row>
-    <row r="42" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="21"/>
+      <c r="K41" s="79"/>
+    </row>
+    <row r="42" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="79"/>
       <c r="B42" s="21">
         <v>33</v>
@@ -20689,13 +20756,14 @@
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="21"/>
+      <c r="I42" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="79"/>
-    </row>
-    <row r="43" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="21"/>
+      <c r="K42" s="79"/>
+    </row>
+    <row r="43" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="79"/>
       <c r="B43" s="21">
         <v>34</v>
@@ -20711,13 +20779,14 @@
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="21"/>
+      <c r="I43" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="79"/>
-    </row>
-    <row r="44" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="21"/>
+      <c r="K43" s="79"/>
+    </row>
+    <row r="44" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="79"/>
       <c r="B44" s="21">
         <v>35</v>
@@ -20733,13 +20802,14 @@
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="21"/>
+      <c r="I44" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="79"/>
-    </row>
-    <row r="45" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="21"/>
+      <c r="K44" s="79"/>
+    </row>
+    <row r="45" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="79"/>
       <c r="B45" s="21">
         <v>36</v>
@@ -20755,13 +20825,14 @@
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="21"/>
+      <c r="I45" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="79"/>
-    </row>
-    <row r="46" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="21"/>
+      <c r="K45" s="79"/>
+    </row>
+    <row r="46" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="79"/>
       <c r="B46" s="21">
         <v>37</v>
@@ -20777,13 +20848,14 @@
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="21"/>
+      <c r="I46" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="79"/>
-    </row>
-    <row r="47" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="21"/>
+      <c r="K46" s="79"/>
+    </row>
+    <row r="47" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="79"/>
       <c r="B47" s="21">
         <v>38</v>
@@ -20799,13 +20871,14 @@
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="21"/>
+      <c r="I47" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="I47" s="21"/>
-      <c r="J47" s="79"/>
-    </row>
-    <row r="48" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="21"/>
+      <c r="K47" s="79"/>
+    </row>
+    <row r="48" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="79"/>
       <c r="B48" s="21">
         <v>39</v>
@@ -20821,13 +20894,14 @@
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="21"/>
+      <c r="I48" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I48" s="21"/>
-      <c r="J48" s="79"/>
-    </row>
-    <row r="49" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="21"/>
+      <c r="K48" s="79"/>
+    </row>
+    <row r="49" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="79"/>
       <c r="B49" s="21">
         <v>40</v>
@@ -20843,13 +20917,14 @@
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="21" t="s">
+      <c r="H49" s="21"/>
+      <c r="I49" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="79"/>
-    </row>
-    <row r="50" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="21"/>
+      <c r="K49" s="79"/>
+    </row>
+    <row r="50" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="79"/>
       <c r="B50" s="21">
         <v>41</v>
@@ -20865,13 +20940,14 @@
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
-      <c r="H50" s="21" t="s">
+      <c r="H50" s="21"/>
+      <c r="I50" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="79"/>
-    </row>
-    <row r="51" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="21"/>
+      <c r="K50" s="79"/>
+    </row>
+    <row r="51" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="79"/>
       <c r="B51" s="21">
         <v>42</v>
@@ -20887,13 +20963,14 @@
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
-      <c r="H51" s="21" t="s">
+      <c r="H51" s="21"/>
+      <c r="I51" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="79"/>
-    </row>
-    <row r="52" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="21"/>
+      <c r="K51" s="79"/>
+    </row>
+    <row r="52" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="79"/>
       <c r="B52" s="21">
         <v>43</v>
@@ -20909,13 +20986,14 @@
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
-      <c r="H52" s="21" t="s">
+      <c r="H52" s="21"/>
+      <c r="I52" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="I52" s="21"/>
-      <c r="J52" s="79"/>
-    </row>
-    <row r="53" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="21"/>
+      <c r="K52" s="79"/>
+    </row>
+    <row r="53" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="79"/>
       <c r="B53" s="21">
         <v>44</v>
@@ -20931,13 +21009,14 @@
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
-      <c r="H53" s="21" t="s">
+      <c r="H53" s="21"/>
+      <c r="I53" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="79"/>
-    </row>
-    <row r="54" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="21"/>
+      <c r="K53" s="79"/>
+    </row>
+    <row r="54" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="79"/>
       <c r="B54" s="21">
         <v>45</v>
@@ -20953,13 +21032,14 @@
       </c>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
-      <c r="H54" s="21" t="s">
+      <c r="H54" s="21"/>
+      <c r="I54" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="79"/>
-    </row>
-    <row r="55" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="21"/>
+      <c r="K54" s="79"/>
+    </row>
+    <row r="55" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="79"/>
       <c r="B55" s="21">
         <v>46</v>
@@ -20975,13 +21055,14 @@
       </c>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
-      <c r="H55" s="21" t="s">
+      <c r="H55" s="21"/>
+      <c r="I55" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="79"/>
-    </row>
-    <row r="56" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="21"/>
+      <c r="K55" s="79"/>
+    </row>
+    <row r="56" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="79"/>
       <c r="B56" s="21">
         <v>47</v>
@@ -20997,13 +21078,14 @@
       </c>
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
-      <c r="H56" s="21" t="s">
+      <c r="H56" s="21"/>
+      <c r="I56" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I56" s="21"/>
-      <c r="J56" s="79"/>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="21"/>
+      <c r="K56" s="79"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
@@ -21011,11 +21093,12 @@
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
-      <c r="H57" s="9"/>
+      <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -21026,8 +21109,9 @@
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -21038,8 +21122,9 @@
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -21050,8 +21135,9 @@
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -21062,15 +21148,16 @@
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="E6:K6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -21116,12 +21203,12 @@
       <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -21132,11 +21219,11 @@
         <v>8</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
@@ -21146,12 +21233,12 @@
       <c r="D6" s="34">
         <v>7</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
@@ -21517,12 +21604,12 @@
       <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
@@ -21533,11 +21620,11 @@
         <v>9</v>
       </c>
       <c r="E5" s="44"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
@@ -21547,12 +21634,12 @@
       <c r="D6" s="47">
         <v>28</v>
       </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="45"/>
@@ -22264,12 +22351,12 @@
       <c r="D4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="88"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
@@ -22281,11 +22368,11 @@
         <v>10</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
@@ -22296,14 +22383,14 @@
       <c r="D6" s="23">
         <v>123</v>
       </c>
-      <c r="E6" s="88" t="s">
+      <c r="E6" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
@@ -25113,12 +25200,12 @@
       <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -25129,11 +25216,11 @@
         <v>12</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
@@ -25143,12 +25230,12 @@
       <c r="D6" s="13">
         <v>39</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
@@ -26905,12 +26992,12 @@
       <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -26921,11 +27008,11 @@
         <v>13</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
@@ -26935,12 +27022,12 @@
       <c r="D6" s="34">
         <v>29</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -27654,12 +27741,12 @@
       <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="40" t="s">
@@ -27670,11 +27757,11 @@
         <v>14</v>
       </c>
       <c r="E5" s="58"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
@@ -27684,12 +27771,12 @@
       <c r="D6" s="14">
         <v>170</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
@@ -31252,25 +31339,25 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -31278,12 +31365,12 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Se añadio una columna en el excel "Fecha Plantaje"
</commit_message>
<xml_diff>
--- a/planilla de almendras para QR.xlsx
+++ b/planilla de almendras para QR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\APK QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577862FC-0486-4A3F-B2BF-6D08BF3D24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C7580-68E3-4519-AC6F-1794DE8C3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="485">
   <si>
     <t>Resumen de las comunidades - Productores y numero de plantas georeferenciadas.</t>
   </si>
@@ -1480,14 +1480,18 @@
   </si>
   <si>
     <t>CA_JB_170</t>
+  </si>
+  <si>
+    <t>Fecha Plantaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1897,7 +1901,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2082,7 +2086,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2101,6 +2111,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2125,7 +2138,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2165,7 +2178,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2205,7 +2218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2245,7 +2258,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2285,7 +2298,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2325,7 +2338,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2365,7 +2378,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2405,7 +2418,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2445,7 +2458,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2485,7 +2498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2525,7 +2538,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2565,7 +2578,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2605,7 +2618,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2645,7 +2658,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2685,7 +2698,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2725,7 +2738,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2765,7 +2778,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2805,7 +2818,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2845,7 +2858,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2885,7 +2898,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2925,7 +2938,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -2965,7 +2978,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3005,7 +3018,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3045,7 +3058,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3085,7 +3098,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3125,7 +3138,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3165,7 +3178,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3205,7 +3218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3245,7 +3258,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3285,7 +3298,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3325,7 +3338,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3365,7 +3378,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3405,7 +3418,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3445,7 +3458,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3485,7 +3498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3525,7 +3538,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3565,7 +3578,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3605,7 +3618,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3645,7 +3658,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3685,7 +3698,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3725,7 +3738,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3765,7 +3778,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3805,7 +3818,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3845,7 +3858,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3885,7 +3898,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3925,7 +3938,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
@@ -3965,7 +3978,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>214313</xdr:rowOff>
@@ -19814,10 +19827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:J61"/>
+  <dimension ref="A2:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19826,14 +19839,14 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="48.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="5" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -19844,8 +19857,9 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -19856,8 +19870,9 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="13" t="s">
         <v>16</v>
@@ -19866,14 +19881,15 @@
       <c r="D4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="88"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="24" t="s">
         <v>17</v>
@@ -19883,13 +19899,14 @@
         <v>6</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="84"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="88"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="13" t="s">
         <v>18</v>
@@ -19898,14 +19915,15 @@
       <c r="D6" s="13">
         <v>47</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="85"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -19915,13 +19933,14 @@
       <c r="E7" s="27">
         <v>8314</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -19932,8 +19951,9 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="30" t="s">
         <v>20</v>
@@ -19948,20 +19968,23 @@
         <v>23</v>
       </c>
       <c r="F9" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="H9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="I9" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="78" t="s">
+      <c r="J9" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79"/>
       <c r="B10" s="28">
         <v>1</v>
@@ -19975,19 +19998,22 @@
       <c r="E10" s="28">
         <v>8314823</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="94">
+        <v>45485</v>
+      </c>
+      <c r="G10" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="79"/>
-    </row>
-    <row r="11" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="60"/>
+      <c r="K10" s="79"/>
+    </row>
+    <row r="11" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79"/>
       <c r="B11" s="21">
         <v>2</v>
@@ -20001,17 +20027,20 @@
       <c r="E11" s="21">
         <v>8314823</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="94">
+        <v>45486</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="60"/>
-      <c r="J11" s="79"/>
-    </row>
-    <row r="12" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="60"/>
+      <c r="K11" s="79"/>
+    </row>
+    <row r="12" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79"/>
       <c r="B12" s="21">
         <v>3</v>
@@ -20025,17 +20054,20 @@
       <c r="E12" s="21">
         <v>8314821</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21" t="s">
+      <c r="F12" s="94">
+        <v>45487</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="I12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="79"/>
-    </row>
-    <row r="13" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="60"/>
+      <c r="K12" s="79"/>
+    </row>
+    <row r="13" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79"/>
       <c r="B13" s="21">
         <v>4</v>
@@ -20049,15 +20081,18 @@
       <c r="E13" s="21">
         <v>8314821</v>
       </c>
-      <c r="F13" s="21"/>
+      <c r="F13" s="94">
+        <v>45488</v>
+      </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="60"/>
-      <c r="J13" s="79"/>
-    </row>
-    <row r="14" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="60"/>
+      <c r="K13" s="79"/>
+    </row>
+    <row r="14" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="79"/>
       <c r="B14" s="21">
         <v>5</v>
@@ -20071,15 +20106,18 @@
       <c r="E14" s="21">
         <v>8314820</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="94">
+        <v>45489</v>
+      </c>
       <c r="G14" s="21"/>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="79"/>
-    </row>
-    <row r="15" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="60"/>
+      <c r="K14" s="79"/>
+    </row>
+    <row r="15" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="79"/>
       <c r="B15" s="21">
         <v>6</v>
@@ -20093,15 +20131,18 @@
       <c r="E15" s="21">
         <v>8314819</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="84">
+        <v>45490</v>
+      </c>
       <c r="G15" s="21"/>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="21"/>
+      <c r="I15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="60"/>
-      <c r="J15" s="79"/>
-    </row>
-    <row r="16" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="60"/>
+      <c r="K15" s="79"/>
+    </row>
+    <row r="16" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="79"/>
       <c r="B16" s="21">
         <v>7</v>
@@ -20117,13 +20158,14 @@
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="79"/>
-    </row>
-    <row r="17" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="60"/>
+      <c r="K16" s="79"/>
+    </row>
+    <row r="17" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="79"/>
       <c r="B17" s="21">
         <v>8</v>
@@ -20139,13 +20181,14 @@
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="60"/>
-      <c r="J17" s="79"/>
-    </row>
-    <row r="18" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="60"/>
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="79"/>
       <c r="B18" s="21">
         <v>9</v>
@@ -20161,13 +20204,14 @@
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="21"/>
+      <c r="I18" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="79"/>
-    </row>
-    <row r="19" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="60"/>
+      <c r="K18" s="79"/>
+    </row>
+    <row r="19" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="79"/>
       <c r="B19" s="21">
         <v>10</v>
@@ -20183,13 +20227,14 @@
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="79"/>
-    </row>
-    <row r="20" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="21"/>
+      <c r="K19" s="79"/>
+    </row>
+    <row r="20" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="79"/>
       <c r="B20" s="21">
         <v>11</v>
@@ -20205,13 +20250,14 @@
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="21"/>
+      <c r="I20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="79"/>
-    </row>
-    <row r="21" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="21"/>
+      <c r="K20" s="79"/>
+    </row>
+    <row r="21" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="79"/>
       <c r="B21" s="21">
         <v>12</v>
@@ -20227,13 +20273,14 @@
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="21"/>
+      <c r="I21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="79"/>
-    </row>
-    <row r="22" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="21"/>
+      <c r="K21" s="79"/>
+    </row>
+    <row r="22" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="79"/>
       <c r="B22" s="21">
         <v>13</v>
@@ -20249,13 +20296,14 @@
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="21"/>
+      <c r="I22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="79"/>
-    </row>
-    <row r="23" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="21"/>
+      <c r="K22" s="79"/>
+    </row>
+    <row r="23" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="79"/>
       <c r="B23" s="21">
         <v>14</v>
@@ -20271,13 +20319,14 @@
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="21"/>
+      <c r="I23" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="79"/>
-    </row>
-    <row r="24" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="21"/>
+      <c r="K23" s="79"/>
+    </row>
+    <row r="24" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="79"/>
       <c r="B24" s="21">
         <v>15</v>
@@ -20293,13 +20342,14 @@
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="21"/>
+      <c r="I24" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="79"/>
-    </row>
-    <row r="25" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="21"/>
+      <c r="K24" s="79"/>
+    </row>
+    <row r="25" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="79"/>
       <c r="B25" s="21">
         <v>16</v>
@@ -20315,13 +20365,14 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="21"/>
+      <c r="I25" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="79"/>
-    </row>
-    <row r="26" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="21"/>
+      <c r="K25" s="79"/>
+    </row>
+    <row r="26" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="79"/>
       <c r="B26" s="21">
         <v>17</v>
@@ -20337,13 +20388,14 @@
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="21"/>
+      <c r="I26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="21"/>
-      <c r="J26" s="79"/>
-    </row>
-    <row r="27" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="21"/>
+      <c r="K26" s="79"/>
+    </row>
+    <row r="27" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="79"/>
       <c r="B27" s="21">
         <v>18</v>
@@ -20359,13 +20411,14 @@
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="21"/>
+      <c r="I27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="79"/>
-    </row>
-    <row r="28" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="21"/>
+      <c r="K27" s="79"/>
+    </row>
+    <row r="28" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="79"/>
       <c r="B28" s="21">
         <v>19</v>
@@ -20381,13 +20434,14 @@
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="21"/>
+      <c r="I28" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="79"/>
-    </row>
-    <row r="29" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="21"/>
+      <c r="K28" s="79"/>
+    </row>
+    <row r="29" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="79"/>
       <c r="B29" s="21">
         <v>20</v>
@@ -20403,13 +20457,14 @@
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="21"/>
+      <c r="I29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="79"/>
-    </row>
-    <row r="30" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="21"/>
+      <c r="K29" s="79"/>
+    </row>
+    <row r="30" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="79"/>
       <c r="B30" s="21">
         <v>21</v>
@@ -20425,13 +20480,14 @@
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="21"/>
+      <c r="I30" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="79"/>
-    </row>
-    <row r="31" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="21"/>
+      <c r="K30" s="79"/>
+    </row>
+    <row r="31" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="79"/>
       <c r="B31" s="21">
         <v>22</v>
@@ -20447,13 +20503,14 @@
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="21"/>
+      <c r="I31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="79"/>
-    </row>
-    <row r="32" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="21"/>
+      <c r="K31" s="79"/>
+    </row>
+    <row r="32" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="79"/>
       <c r="B32" s="21">
         <v>23</v>
@@ -20469,13 +20526,14 @@
       </c>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="21"/>
+      <c r="I32" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="79"/>
-    </row>
-    <row r="33" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="21"/>
+      <c r="K32" s="79"/>
+    </row>
+    <row r="33" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="79"/>
       <c r="B33" s="21">
         <v>24</v>
@@ -20491,13 +20549,14 @@
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="21"/>
+      <c r="I33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="79"/>
-    </row>
-    <row r="34" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="21"/>
+      <c r="K33" s="79"/>
+    </row>
+    <row r="34" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="79"/>
       <c r="B34" s="21">
         <v>25</v>
@@ -20513,13 +20572,14 @@
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="21"/>
+      <c r="I34" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="79"/>
-    </row>
-    <row r="35" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="21"/>
+      <c r="K34" s="79"/>
+    </row>
+    <row r="35" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="79"/>
       <c r="B35" s="21">
         <v>26</v>
@@ -20535,13 +20595,14 @@
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="21"/>
+      <c r="I35" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="79"/>
-    </row>
-    <row r="36" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="21"/>
+      <c r="K35" s="79"/>
+    </row>
+    <row r="36" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="79"/>
       <c r="B36" s="21">
         <v>27</v>
@@ -20557,13 +20618,14 @@
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="21"/>
+      <c r="I36" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="79"/>
-    </row>
-    <row r="37" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="21"/>
+      <c r="K36" s="79"/>
+    </row>
+    <row r="37" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="79"/>
       <c r="B37" s="21">
         <v>28</v>
@@ -20579,13 +20641,14 @@
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="21" t="s">
+      <c r="H37" s="21"/>
+      <c r="I37" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="79"/>
-    </row>
-    <row r="38" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="21"/>
+      <c r="K37" s="79"/>
+    </row>
+    <row r="38" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="79"/>
       <c r="B38" s="21">
         <v>29</v>
@@ -20601,13 +20664,14 @@
       </c>
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="21"/>
+      <c r="I38" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="79"/>
-    </row>
-    <row r="39" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="21"/>
+      <c r="K38" s="79"/>
+    </row>
+    <row r="39" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="79"/>
       <c r="B39" s="21">
         <v>30</v>
@@ -20623,13 +20687,14 @@
       </c>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="21"/>
+      <c r="I39" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="79"/>
-    </row>
-    <row r="40" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="21"/>
+      <c r="K39" s="79"/>
+    </row>
+    <row r="40" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="79"/>
       <c r="B40" s="21">
         <v>31</v>
@@ -20645,13 +20710,14 @@
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="21"/>
+      <c r="I40" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="21"/>
-      <c r="J40" s="79"/>
-    </row>
-    <row r="41" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="21"/>
+      <c r="K40" s="79"/>
+    </row>
+    <row r="41" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="79"/>
       <c r="B41" s="21">
         <v>32</v>
@@ -20667,13 +20733,14 @@
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="21"/>
+      <c r="I41" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="79"/>
-    </row>
-    <row r="42" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="21"/>
+      <c r="K41" s="79"/>
+    </row>
+    <row r="42" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="79"/>
       <c r="B42" s="21">
         <v>33</v>
@@ -20689,13 +20756,14 @@
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="21"/>
+      <c r="I42" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="79"/>
-    </row>
-    <row r="43" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="21"/>
+      <c r="K42" s="79"/>
+    </row>
+    <row r="43" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="79"/>
       <c r="B43" s="21">
         <v>34</v>
@@ -20711,13 +20779,14 @@
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="21"/>
+      <c r="I43" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="79"/>
-    </row>
-    <row r="44" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="21"/>
+      <c r="K43" s="79"/>
+    </row>
+    <row r="44" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="79"/>
       <c r="B44" s="21">
         <v>35</v>
@@ -20733,13 +20802,14 @@
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="21"/>
+      <c r="I44" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="79"/>
-    </row>
-    <row r="45" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="21"/>
+      <c r="K44" s="79"/>
+    </row>
+    <row r="45" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="79"/>
       <c r="B45" s="21">
         <v>36</v>
@@ -20755,13 +20825,14 @@
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="21"/>
+      <c r="I45" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="79"/>
-    </row>
-    <row r="46" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="21"/>
+      <c r="K45" s="79"/>
+    </row>
+    <row r="46" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="79"/>
       <c r="B46" s="21">
         <v>37</v>
@@ -20777,13 +20848,14 @@
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="21"/>
+      <c r="I46" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="79"/>
-    </row>
-    <row r="47" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="21"/>
+      <c r="K46" s="79"/>
+    </row>
+    <row r="47" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="79"/>
       <c r="B47" s="21">
         <v>38</v>
@@ -20799,13 +20871,14 @@
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="21" t="s">
+      <c r="H47" s="21"/>
+      <c r="I47" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="I47" s="21"/>
-      <c r="J47" s="79"/>
-    </row>
-    <row r="48" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="21"/>
+      <c r="K47" s="79"/>
+    </row>
+    <row r="48" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="79"/>
       <c r="B48" s="21">
         <v>39</v>
@@ -20821,13 +20894,14 @@
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
-      <c r="H48" s="21" t="s">
+      <c r="H48" s="21"/>
+      <c r="I48" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I48" s="21"/>
-      <c r="J48" s="79"/>
-    </row>
-    <row r="49" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="21"/>
+      <c r="K48" s="79"/>
+    </row>
+    <row r="49" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="79"/>
       <c r="B49" s="21">
         <v>40</v>
@@ -20843,13 +20917,14 @@
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="21" t="s">
+      <c r="H49" s="21"/>
+      <c r="I49" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="79"/>
-    </row>
-    <row r="50" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="21"/>
+      <c r="K49" s="79"/>
+    </row>
+    <row r="50" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="79"/>
       <c r="B50" s="21">
         <v>41</v>
@@ -20865,13 +20940,14 @@
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
-      <c r="H50" s="21" t="s">
+      <c r="H50" s="21"/>
+      <c r="I50" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="79"/>
-    </row>
-    <row r="51" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="21"/>
+      <c r="K50" s="79"/>
+    </row>
+    <row r="51" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="79"/>
       <c r="B51" s="21">
         <v>42</v>
@@ -20887,13 +20963,14 @@
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
-      <c r="H51" s="21" t="s">
+      <c r="H51" s="21"/>
+      <c r="I51" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="79"/>
-    </row>
-    <row r="52" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="21"/>
+      <c r="K51" s="79"/>
+    </row>
+    <row r="52" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="79"/>
       <c r="B52" s="21">
         <v>43</v>
@@ -20909,13 +20986,14 @@
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
-      <c r="H52" s="21" t="s">
+      <c r="H52" s="21"/>
+      <c r="I52" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="I52" s="21"/>
-      <c r="J52" s="79"/>
-    </row>
-    <row r="53" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="21"/>
+      <c r="K52" s="79"/>
+    </row>
+    <row r="53" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="79"/>
       <c r="B53" s="21">
         <v>44</v>
@@ -20931,13 +21009,14 @@
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
-      <c r="H53" s="21" t="s">
+      <c r="H53" s="21"/>
+      <c r="I53" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="79"/>
-    </row>
-    <row r="54" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="21"/>
+      <c r="K53" s="79"/>
+    </row>
+    <row r="54" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="79"/>
       <c r="B54" s="21">
         <v>45</v>
@@ -20953,13 +21032,14 @@
       </c>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
-      <c r="H54" s="21" t="s">
+      <c r="H54" s="21"/>
+      <c r="I54" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="79"/>
-    </row>
-    <row r="55" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="21"/>
+      <c r="K54" s="79"/>
+    </row>
+    <row r="55" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="79"/>
       <c r="B55" s="21">
         <v>46</v>
@@ -20975,13 +21055,14 @@
       </c>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
-      <c r="H55" s="21" t="s">
+      <c r="H55" s="21"/>
+      <c r="I55" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="79"/>
-    </row>
-    <row r="56" spans="1:10" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="21"/>
+      <c r="K55" s="79"/>
+    </row>
+    <row r="56" spans="1:11" s="61" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="79"/>
       <c r="B56" s="21">
         <v>47</v>
@@ -20997,13 +21078,14 @@
       </c>
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
-      <c r="H56" s="21" t="s">
+      <c r="H56" s="21"/>
+      <c r="I56" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I56" s="21"/>
-      <c r="J56" s="79"/>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="21"/>
+      <c r="K56" s="79"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
@@ -21011,11 +21093,12 @@
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
-      <c r="H57" s="9"/>
+      <c r="H57" s="11"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -21026,8 +21109,9 @@
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -21038,8 +21122,9 @@
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -21050,8 +21135,9 @@
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -21062,15 +21148,16 @@
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="E6:K6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -21116,12 +21203,12 @@
       <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -21132,11 +21219,11 @@
         <v>8</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
@@ -21146,12 +21233,12 @@
       <c r="D6" s="34">
         <v>7</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
@@ -21517,12 +21604,12 @@
       <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
@@ -21533,11 +21620,11 @@
         <v>9</v>
       </c>
       <c r="E5" s="44"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
@@ -21547,12 +21634,12 @@
       <c r="D6" s="47">
         <v>28</v>
       </c>
-      <c r="E6" s="87"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="45"/>
@@ -22264,12 +22351,12 @@
       <c r="D4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="88"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
@@ -22281,11 +22368,11 @@
         <v>10</v>
       </c>
       <c r="E5" s="53"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
@@ -22296,14 +22383,14 @@
       <c r="D6" s="23">
         <v>123</v>
       </c>
-      <c r="E6" s="88" t="s">
+      <c r="E6" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
@@ -25113,12 +25200,12 @@
       <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -25129,11 +25216,11 @@
         <v>12</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
@@ -25143,12 +25230,12 @@
       <c r="D6" s="13">
         <v>39</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
@@ -26905,12 +26992,12 @@
       <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
@@ -26921,11 +27008,11 @@
         <v>13</v>
       </c>
       <c r="E5" s="26"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
@@ -26935,12 +27022,12 @@
       <c r="D6" s="34">
         <v>29</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
@@ -27654,12 +27741,12 @@
       <c r="D4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="40" t="s">
@@ -27670,11 +27757,11 @@
         <v>14</v>
       </c>
       <c r="E5" s="58"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
@@ -27684,12 +27771,12 @@
       <c r="D6" s="14">
         <v>170</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
@@ -31252,25 +31339,25 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="86"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
     </row>
     <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -31278,12 +31365,12 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="86"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="88"/>
     </row>
     <row r="7" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>

</xml_diff>